<commit_message>
Fixed a typo in the confi
</commit_message>
<xml_diff>
--- a/database-advanced-zb0142/config.xlsx
+++ b/database-advanced-zb0142/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\canvas-course-scaffolder-with-course-configs\database-advanced-zb0142\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFF3D70B-081F-4A39-A75B-89800E4120CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFDD54B6-D270-4D21-BE1D-68D02FEEE9B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27708" windowHeight="16560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Algemene info" sheetId="1" r:id="rId1"/>
@@ -165,9 +165,6 @@
     <t>Kristine Mangelschots, Sebastiaan Henau</t>
   </si>
   <si>
-    <t>kristine.mangelschots@thomasmore.be, sebastiaan.henau@gmail.com</t>
-  </si>
-  <si>
     <t>Database Advanced</t>
   </si>
   <si>
@@ -415,6 +412,9 @@
   </si>
   <si>
     <t>Oplossingen</t>
+  </si>
+  <si>
+    <t>kristine.mangelschots@thomasmore.be, sebastiaan.henau@thomasmore.be</t>
   </si>
 </sst>
 </file>
@@ -520,7 +520,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -909,8 +909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -932,7 +932,7 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -948,7 +948,7 @@
         <v>17</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>39</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -956,7 +956,7 @@
         <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1011,7 +1011,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B4">
         <v>100</v>
@@ -1076,7 +1076,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C2" s="1">
         <v>45443.999305555553</v>
@@ -1094,7 +1094,7 @@
         <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -1201,10 +1201,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -1263,7 +1263,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1271,7 +1271,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1279,7 +1279,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -1287,7 +1287,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -1295,7 +1295,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -1303,7 +1303,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -1311,7 +1311,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -1319,7 +1319,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -1327,7 +1327,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -1335,7 +1335,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -1343,7 +1343,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -1351,7 +1351,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -1359,7 +1359,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -1378,7 +1378,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E63DFD8-2013-40A2-8CE5-0CB5ABE5CD54}">
   <dimension ref="A1:I64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+    <sheetView topLeftCell="A40" workbookViewId="0">
       <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
@@ -1426,13 +1426,13 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -1443,47 +1443,47 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" t="s">
         <v>51</v>
-      </c>
-      <c r="C7" t="s">
-        <v>52</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -1494,19 +1494,19 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" t="s">
         <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I8">
         <v>1</v>
@@ -1514,13 +1514,13 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -1531,19 +1531,19 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B10" t="s">
         <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I10">
         <v>1</v>
@@ -1551,19 +1551,19 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B11" t="s">
         <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D11">
         <v>0</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I11">
         <v>2</v>
@@ -1571,19 +1571,19 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B12" t="s">
         <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D12">
         <v>0</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I12">
         <v>2</v>
@@ -1591,13 +1591,13 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" t="s">
         <v>51</v>
-      </c>
-      <c r="C14" t="s">
-        <v>52</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -1608,19 +1608,19 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B15" t="s">
         <v>34</v>
       </c>
       <c r="C15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
       <c r="F15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I15">
         <v>1</v>
@@ -1628,13 +1628,13 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -1645,19 +1645,19 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B17" t="s">
         <v>34</v>
       </c>
       <c r="C17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I17">
         <v>1</v>
@@ -1665,19 +1665,19 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B18" t="s">
         <v>34</v>
       </c>
       <c r="C18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D18">
         <v>0</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I18">
         <v>2</v>
@@ -1685,19 +1685,19 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B19" t="s">
         <v>34</v>
       </c>
       <c r="C19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D19">
         <v>0</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I19">
         <v>2</v>
@@ -1705,13 +1705,13 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B21" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="7" t="s">
         <v>51</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>52</v>
       </c>
       <c r="D21" s="7">
         <v>1</v>
@@ -1726,20 +1726,20 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D22" s="4">
         <v>1</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
@@ -1749,13 +1749,13 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D23" s="7">
         <v>1</v>
@@ -1770,20 +1770,20 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D24" s="4">
         <v>1</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
@@ -1793,20 +1793,20 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>34</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D25" s="7">
         <v>0</v>
       </c>
       <c r="E25" s="7"/>
       <c r="F25" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G25" s="7"/>
       <c r="H25" s="7"/>
@@ -1816,20 +1816,20 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D26" s="4">
         <v>0</v>
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
@@ -1839,13 +1839,13 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D28" s="7">
         <v>1</v>
@@ -1860,20 +1860,20 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D29" s="4">
         <v>1</v>
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
@@ -1883,20 +1883,20 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>34</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D30" s="7">
         <v>0</v>
       </c>
       <c r="E30" s="7"/>
       <c r="F30" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G30" s="7"/>
       <c r="H30" s="7"/>
@@ -1906,20 +1906,20 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B31" s="7" t="s">
         <v>34</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D31" s="7">
         <v>0</v>
       </c>
       <c r="E31" s="7"/>
       <c r="F31" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G31" s="7"/>
       <c r="H31" s="7"/>
@@ -1929,20 +1929,20 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D32" s="4">
         <v>0</v>
       </c>
       <c r="E32" s="4"/>
       <c r="F32" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
@@ -1952,13 +1952,13 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B34" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C34" s="7" t="s">
         <v>51</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>52</v>
       </c>
       <c r="D34" s="7">
         <v>1</v>
@@ -1973,20 +1973,20 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D35" s="4">
         <v>1</v>
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
@@ -1996,13 +1996,13 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D36" s="7">
         <v>1</v>
@@ -2017,20 +2017,20 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D37" s="4">
         <v>1</v>
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G37" s="4"/>
       <c r="H37" s="4"/>
@@ -2040,20 +2040,20 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>34</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D38" s="7">
         <v>0</v>
       </c>
       <c r="E38" s="7"/>
       <c r="F38" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G38" s="7"/>
       <c r="H38" s="7"/>
@@ -2063,20 +2063,20 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D39" s="4">
         <v>0</v>
       </c>
       <c r="E39" s="4"/>
       <c r="F39" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G39" s="4"/>
       <c r="H39" s="4"/>
@@ -2097,13 +2097,13 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D41" s="7">
         <v>1</v>
@@ -2118,20 +2118,20 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D42" s="4">
         <v>1</v>
       </c>
       <c r="E42" s="4"/>
       <c r="F42" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G42" s="4"/>
       <c r="H42" s="4"/>
@@ -2141,20 +2141,20 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B43" s="7" t="s">
         <v>34</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D43" s="7">
         <v>0</v>
       </c>
       <c r="E43" s="7"/>
       <c r="F43" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G43" s="7"/>
       <c r="H43" s="7"/>
@@ -2164,20 +2164,20 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D44" s="4">
         <v>0</v>
       </c>
       <c r="E44" s="4"/>
       <c r="F44" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G44" s="4"/>
       <c r="H44" s="4"/>
@@ -2187,13 +2187,13 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B46" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C46" s="7" t="s">
         <v>51</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>52</v>
       </c>
       <c r="D46" s="7">
         <v>0</v>
@@ -2208,20 +2208,20 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D47" s="4">
         <v>0</v>
       </c>
       <c r="E47" s="4"/>
       <c r="F47" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G47" s="4"/>
       <c r="H47" s="4"/>
@@ -2231,13 +2231,13 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D48" s="7">
         <v>0</v>
@@ -2252,20 +2252,20 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D49" s="4">
         <v>0</v>
       </c>
       <c r="E49" s="4"/>
       <c r="F49" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G49" s="4"/>
       <c r="H49" s="4"/>
@@ -2275,20 +2275,20 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B50" s="7" t="s">
         <v>34</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D50" s="7">
         <v>0</v>
       </c>
       <c r="E50" s="7"/>
       <c r="F50" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G50" s="7"/>
       <c r="H50" s="7"/>
@@ -2298,20 +2298,20 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D51" s="4">
         <v>0</v>
       </c>
       <c r="E51" s="4"/>
       <c r="F51" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G51" s="4"/>
       <c r="H51" s="4"/>
@@ -2321,13 +2321,13 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B53" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C53" s="7" t="s">
         <v>51</v>
-      </c>
-      <c r="C53" s="7" t="s">
-        <v>52</v>
       </c>
       <c r="D53" s="7">
         <v>0</v>
@@ -2342,20 +2342,20 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D54" s="4">
         <v>0</v>
       </c>
       <c r="E54" s="4"/>
       <c r="F54" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G54" s="4"/>
       <c r="H54" s="4"/>
@@ -2365,13 +2365,13 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D55" s="7">
         <v>0</v>
@@ -2386,20 +2386,20 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D56" s="4">
         <v>0</v>
       </c>
       <c r="E56" s="4"/>
       <c r="F56" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G56" s="4"/>
       <c r="H56" s="4"/>
@@ -2409,20 +2409,20 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B57" s="7" t="s">
         <v>34</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D57" s="7">
         <v>0</v>
       </c>
       <c r="E57" s="7"/>
       <c r="F57" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G57" s="7"/>
       <c r="H57" s="7"/>
@@ -2432,20 +2432,20 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D58" s="4">
         <v>0</v>
       </c>
       <c r="E58" s="4"/>
       <c r="F58" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G58" s="4"/>
       <c r="H58" s="4"/>
@@ -2455,13 +2455,13 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D60" s="7">
         <v>1</v>
@@ -2476,20 +2476,20 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B61" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D61" s="4">
         <v>1</v>
       </c>
       <c r="E61" s="4"/>
       <c r="F61" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G61" s="4"/>
       <c r="H61" s="4"/>
@@ -2499,20 +2499,20 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B63" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D63" s="4">
         <v>1</v>
       </c>
       <c r="E63" s="4"/>
       <c r="F63" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G63" s="4"/>
       <c r="H63" s="4"/>
@@ -2522,20 +2522,20 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B64" s="7" t="s">
         <v>34</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D64" s="7">
         <v>0</v>
       </c>
       <c r="E64" s="7"/>
       <c r="F64" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G64" s="7"/>
       <c r="H64" s="7"/>

</xml_diff>